<commit_message>
dist changes check for state - live or frozen
</commit_message>
<xml_diff>
--- a/RME_Rail_Fares/dist/RME_webscrape/Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/RME_Rail_Fares/dist/RME_webscrape/Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\RME_Rail_Fares\dist\RME_webscrape\Route_and_times_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>Route7</t>
+  </si>
+  <si>
+    <t>PAD,BRI</t>
+  </si>
+  <si>
+    <t>BRI,PAD</t>
+  </si>
+  <si>
+    <t>0900,1000</t>
   </si>
 </sst>
 </file>
@@ -500,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +527,7 @@
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -537,8 +549,11 @@
       <c r="G1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -560,8 +575,11 @@
       <c r="G2" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -583,8 +601,11 @@
       <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -606,8 +627,11 @@
       <c r="G4" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -629,8 +653,11 @@
       <c r="G5" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -652,8 +679,11 @@
       <c r="G6" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -675,8 +705,11 @@
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -698,8 +731,11 @@
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -720,6 +756,9 @@
       </c>
       <c r="G9" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>